<commit_message>
Updated order and icon path
</commit_message>
<xml_diff>
--- a/FFL_Data.xlsx
+++ b/FFL_Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelrade\Downloads\FFL-Dash-2023-main\FFL-Dash-2023-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenaxelrad/Desktop/FFL-Dash-2023-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50004792-76CA-43EC-819D-B4166724C0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A785431E-9F47-644E-A0D1-2A5A183934D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1170" windowWidth="19380" windowHeight="12225" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Results" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2023 Results'!$A$41:$B$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2023 Results'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -105,9 +105,6 @@
     <t>Team Icons/brothers-modified.png</t>
   </si>
   <si>
-    <t>Team Icons/jerick-modified.png</t>
-  </si>
-  <si>
     <t>Team Icons/kelce-modified.png</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Ford v Amari</t>
+  </si>
+  <si>
+    <t>Team Icons/ford-modified.png</t>
   </si>
 </sst>
 </file>
@@ -500,19 +500,19 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:XFD92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -529,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -543,7 +543,7 @@
         <v>135.91999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -557,63 +557,63 @@
         <v>90.14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>135.91999999999999</v>
+        <v>84.64</v>
       </c>
       <c r="D4">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>90.2</v>
+        <v>135.91999999999999</v>
       </c>
       <c r="D5">
-        <v>113.54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
+        <v>90.2</v>
+      </c>
+      <c r="D6">
         <v>113.54</v>
       </c>
-      <c r="D6">
-        <v>90.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>84.64</v>
+        <v>113.54</v>
       </c>
       <c r="D7">
-        <v>94.16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -627,7 +627,7 @@
         <v>102.14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -641,7 +641,7 @@
         <v>90.04</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -655,7 +655,7 @@
         <v>82.76</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -669,7 +669,7 @@
         <v>84.64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -683,7 +683,7 @@
         <v>88.48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -697,7 +697,7 @@
         <v>89.96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -711,7 +711,7 @@
         <v>88.06</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -725,63 +725,63 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16">
-        <v>84.8</v>
+        <v>94.76</v>
       </c>
       <c r="D16">
-        <v>119.94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118.64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>123.72</v>
+        <v>84.8</v>
       </c>
       <c r="D17">
-        <v>113.88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18">
-        <v>88.06</v>
+        <v>123.72</v>
       </c>
       <c r="D18">
-        <v>107.34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>113.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>94.76</v>
+        <v>88.06</v>
       </c>
       <c r="D19">
-        <v>118.64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -795,7 +795,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -809,7 +809,7 @@
         <v>123.72</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -823,7 +823,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -837,7 +837,7 @@
         <v>77.180000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -851,7 +851,7 @@
         <v>94.76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -865,7 +865,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -879,7 +879,7 @@
         <v>140.78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -893,63 +893,63 @@
         <v>135.96</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1">
-        <v>62.66</v>
+      <c r="C28">
+        <v>110.92</v>
       </c>
       <c r="D28" s="1">
-        <v>88.7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117.08</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29">
-        <v>140.78</v>
-      </c>
-      <c r="D29">
-        <v>143.66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>62.66</v>
+      </c>
+      <c r="D29" s="1">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30">
-        <v>135.96</v>
-      </c>
-      <c r="D30" s="1">
-        <v>123.46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140.78</v>
+      </c>
+      <c r="D30">
+        <v>143.66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31">
-        <v>110.92</v>
+        <v>135.96</v>
       </c>
       <c r="D31" s="1">
-        <v>117.08</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123.46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -963,7 +963,7 @@
         <v>113.66</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -977,7 +977,7 @@
         <v>110.92</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -991,7 +991,7 @@
         <v>62.66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>109.08</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>112.98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>137.16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>139.04</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1061,63 +1061,63 @@
         <v>82.92</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1">
-        <v>107.44</v>
+        <v>133.30000000000001</v>
       </c>
       <c r="D40" s="1">
-        <v>90.64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112.26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="1">
-        <v>112.26</v>
+        <v>107.44</v>
       </c>
       <c r="D41" s="1">
-        <v>133.30000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="1">
-        <v>87.48</v>
+        <v>112.26</v>
       </c>
       <c r="D42" s="1">
-        <v>123.96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133.30000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="1">
-        <v>133.30000000000001</v>
+        <v>87.48</v>
       </c>
       <c r="D43" s="1">
-        <v>112.26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123.96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>99.24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>87.48</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>107.44</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>103.42</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -1201,12 +1201,12 @@
         <v>84.36</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" s="1">
         <v>111.28</v>
@@ -1215,12 +1215,12 @@
         <v>106.88</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="1">
         <v>79.38</v>
@@ -1229,68 +1229,68 @@
         <v>115.72</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="1">
+        <v>114.36</v>
+      </c>
+      <c r="D52" s="1">
+        <v>108.34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>15</v>
       </c>
-      <c r="B52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="1">
+      <c r="B53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="1">
         <v>88.22</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D53" s="1">
         <v>70.22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>16</v>
       </c>
-      <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="1">
         <v>115.72</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D54" s="1">
         <v>79.38</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>19</v>
       </c>
-      <c r="B54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="1">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="1">
         <v>63.82</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D55" s="1">
         <v>144.34</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="1">
-        <v>114.36</v>
-      </c>
-      <c r="D55" s="1">
-        <v>108.34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" s="1">
         <v>110.14</v>
@@ -1299,12 +1299,12 @@
         <v>110.46</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1">
         <v>110.46</v>
@@ -1313,12 +1313,12 @@
         <v>110.14</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1">
         <v>106.88</v>
@@ -1327,12 +1327,12 @@
         <v>111.28</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="1">
         <v>144.34</v>
@@ -1341,12 +1341,12 @@
         <v>63.82</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" s="1">
         <v>70.22</v>
@@ -1355,12 +1355,12 @@
         <v>88.22</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1">
         <v>108.34</v>
@@ -1369,12 +1369,12 @@
         <v>114.36</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C62" s="1">
         <v>85.2</v>
@@ -1383,12 +1383,12 @@
         <v>99.86</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C63" s="1">
         <v>92.34</v>
@@ -1397,68 +1397,68 @@
         <v>107.68</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="1">
+        <v>98.26</v>
+      </c>
+      <c r="D64" s="1">
+        <v>131.04</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>15</v>
       </c>
-      <c r="B64" t="s">
-        <v>33</v>
-      </c>
-      <c r="C64" s="1">
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="1">
         <v>98.78</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D65" s="1">
         <v>97.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>16</v>
       </c>
-      <c r="B65" t="s">
-        <v>33</v>
-      </c>
-      <c r="C65" s="1">
+      <c r="B66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="1">
         <v>88.1</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D66" s="1">
         <v>86.42</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>19</v>
       </c>
-      <c r="B66" t="s">
-        <v>33</v>
-      </c>
-      <c r="C66" s="1">
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="1">
         <v>109.08</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D67" s="1">
         <v>110.82</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>36</v>
-      </c>
-      <c r="B67" t="s">
-        <v>33</v>
-      </c>
-      <c r="C67" s="1">
-        <v>98.26</v>
-      </c>
-      <c r="D67" s="1">
-        <v>131.04</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1">
         <v>131.04</v>
@@ -1467,12 +1467,12 @@
         <v>98.26</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1">
         <v>97.5</v>
@@ -1481,12 +1481,12 @@
         <v>98.78</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C70" s="1">
         <v>107.68</v>
@@ -1495,12 +1495,12 @@
         <v>92.34</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C71" s="1">
         <v>99.86</v>
@@ -1509,12 +1509,12 @@
         <v>85.2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C72" s="1">
         <v>110.82</v>
@@ -1523,12 +1523,12 @@
         <v>109.08</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C73" s="1">
         <v>86.42</v>
@@ -1537,12 +1537,12 @@
         <v>88.1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C74" s="1">
         <v>77.58</v>
@@ -1551,12 +1551,12 @@
         <v>129.84</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C75" s="1">
         <v>104.4</v>
@@ -1565,68 +1565,68 @@
         <v>85.2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="1">
+        <v>137.19999999999999</v>
+      </c>
+      <c r="D76" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>15</v>
       </c>
-      <c r="B76" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76" s="1">
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="1">
         <v>69</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D77" s="1">
         <v>137.19999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>16</v>
       </c>
-      <c r="B77" t="s">
-        <v>34</v>
-      </c>
-      <c r="C77" s="1">
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="1">
         <v>98.06</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D78" s="1">
         <v>75.16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>19</v>
       </c>
-      <c r="B78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78" s="1">
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="1">
         <v>84.24</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D79" s="1">
         <v>148.41999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>36</v>
-      </c>
-      <c r="B79" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" s="1">
-        <v>137.19999999999999</v>
-      </c>
-      <c r="D79" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C80" s="1">
         <v>119.56</v>
@@ -1635,12 +1635,12 @@
         <v>80.58</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C81" s="1">
         <v>148.41999999999999</v>
@@ -1649,12 +1649,12 @@
         <v>84.24</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C82" s="1">
         <v>75.16</v>
@@ -1663,12 +1663,12 @@
         <v>98.06</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C83" s="1">
         <v>85.2</v>
@@ -1677,12 +1677,12 @@
         <v>104.4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C84" s="1">
         <v>129.84</v>
@@ -1691,12 +1691,12 @@
         <v>77.58</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C85" s="1">
         <v>80.58</v>
@@ -1705,12 +1705,12 @@
         <v>119.56</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C86" s="1">
         <v>100.2</v>
@@ -1722,12 +1722,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C87" s="1">
         <v>130.58000000000001</v>
@@ -1739,80 +1739,80 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" s="1">
+        <v>158.36000000000001</v>
+      </c>
+      <c r="D88" s="1">
+        <v>96.96</v>
+      </c>
+      <c r="E88" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>15</v>
       </c>
-      <c r="B88" t="s">
-        <v>35</v>
-      </c>
-      <c r="C88" s="1">
+      <c r="B89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="1">
         <v>109.06</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D89" s="1">
         <v>101.48</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>16</v>
       </c>
-      <c r="B89" t="s">
-        <v>35</v>
-      </c>
-      <c r="C89" s="1">
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" s="1">
         <v>113.66</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D90" s="1">
         <v>99.34</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E90" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>19</v>
       </c>
-      <c r="B90" t="s">
-        <v>35</v>
-      </c>
-      <c r="C90" s="1">
+      <c r="B91" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="1">
         <v>96.96</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D91" s="1">
         <v>158.36000000000001</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>36</v>
-      </c>
-      <c r="B91" t="s">
-        <v>35</v>
-      </c>
-      <c r="C91" s="1">
-        <v>158.36000000000001</v>
-      </c>
-      <c r="D91" s="1">
-        <v>96.96</v>
-      </c>
-      <c r="E91" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C92" s="1">
         <v>99.34</v>
@@ -1821,15 +1821,15 @@
         <v>113.66</v>
       </c>
       <c r="E92" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C93" s="1">
         <v>119.22</v>
@@ -1838,15 +1838,15 @@
         <v>100.2</v>
       </c>
       <c r="E93" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>13</v>
       </c>
       <c r="B94" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C94" s="1">
         <v>111.42</v>
@@ -1855,15 +1855,15 @@
         <v>99.7</v>
       </c>
       <c r="E94" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C95" s="1">
         <v>99.7</v>
@@ -1872,15 +1872,15 @@
         <v>111.42</v>
       </c>
       <c r="E95" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C96" s="1">
         <v>116.9</v>
@@ -1889,15 +1889,15 @@
         <v>130.58000000000001</v>
       </c>
       <c r="E96" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C97" s="1">
         <v>101.48</v>
@@ -1906,11 +1906,11 @@
         <v>109.06</v>
       </c>
       <c r="E97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A13">
+  <sortState ref="A2:A13">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>